<commit_message>
Modified ImpedanceTest for excel file
</commit_message>
<xml_diff>
--- a/knazarzadeh_ESPM_Pouch_cells_EIS.xlsx
+++ b/knazarzadeh_ESPM_Pouch_cells_EIS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k.nazarzadeh\Projects\EIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529CDF70-628F-4BFA-AE1E-1F3CFA3E59F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C647A44D-B135-42F1-B22A-C07F81081899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="859" activeTab="3" xr2:uid="{D1BE3A99-A2EC-411A-B2ED-F06EA9DB5359}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="859" xr2:uid="{D1BE3A99-A2EC-411A-B2ED-F06EA9DB5359}"/>
   </bookViews>
   <sheets>
     <sheet name="Geometric" sheetId="1" r:id="rId1"/>
@@ -568,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -619,19 +619,9 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -970,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFC985D-5F8A-48FA-B4EF-A05589E05952}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1283,7 +1273,7 @@
       <c r="B19" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="19"/>
+      <c r="C19" s="15"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="6"/>
@@ -1293,7 +1283,7 @@
       <c r="B20" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C20" s="19"/>
+      <c r="C20" s="15"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="6"/>
@@ -1303,7 +1293,7 @@
       <c r="B21" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C21" s="19"/>
+      <c r="C21" s="15"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="6"/>
@@ -1313,7 +1303,7 @@
       <c r="B22" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C22" s="19"/>
+      <c r="C22" s="15"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="6"/>
@@ -1323,7 +1313,7 @@
       <c r="B23" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C23" s="20"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="6"/>
@@ -1906,7 +1896,7 @@
       <c r="B7" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="19"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="6"/>
@@ -2134,7 +2124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F06446-4779-4B39-B482-AB82EC6AA7F7}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -2259,7 +2249,7 @@
       <c r="B8" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="19"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="6"/>
@@ -2269,7 +2259,7 @@
       <c r="B9" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C9" s="19"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="6"/>
@@ -2279,7 +2269,7 @@
       <c r="B10" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C10" s="19"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="6"/>
@@ -2289,7 +2279,7 @@
       <c r="B11" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C11" s="21"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="6"/>
@@ -2299,7 +2289,7 @@
       <c r="B12" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
@@ -2628,7 +2618,7 @@
       <c r="B3" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="20">
         <v>5</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -2737,7 +2727,7 @@
       <c r="B10" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="13">
         <v>0</v>
       </c>
       <c r="D10" s="8" t="s">

</xml_diff>